<commit_message>
?????? ???????? float ? Decimal ????????, ? ??? ?? ????? ??? win.
</commit_message>
<xml_diff>
--- a/src/tests/test_data/linux/test-383.xlsx
+++ b/src/tests/test_data/linux/test-383.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="_xlnm.Print_Titles" vbProcedure="false">{#NAME?}}}}}}</definedName>
+    <definedName function="false" hidden="false" name="_xlnm.Print_Titles" vbProcedure="false">{#NAME?}}}}}}}}</definedName>
     <definedName function="false" hidden="false" name="_xlnm.Print_Titles_1" vbProcedure="false">Лист1!$14:$18</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -674,24 +674,24 @@
   </sheetPr>
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="L4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A4" xSplit="0" ySplit="-1"/>
-      <selection activeCell="C18" activeCellId="0" pane="topLeft" sqref="C18"/>
-      <selection activeCell="A4" activeCellId="0" pane="bottomLeft" sqref="A4"/>
+      <selection activeCell="N12" activeCellId="0" pane="topLeft" sqref="N12"/>
+      <selection activeCell="L4" activeCellId="0" pane="bottomLeft" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.1921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6039215686275"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.23921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4980392156863"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="0.862745098039216"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4196078431373"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4980392156863"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="0.862745098039216"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="11.2980392156863"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.91372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.8156862745098"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="11.3921568627451"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.97647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.88627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="1">
@@ -911,7 +911,7 @@
         <v>21</v>
       </c>
       <c r="N11" s="22" t="n">
-        <v>111</v>
+        <v>10356</v>
       </c>
       <c r="O11" s="22"/>
       <c r="S11" s="6" t="s">

</xml_diff>